<commit_message>
created branch manager module, updated usecase, uploaded to clean list on documentation
</commit_message>
<xml_diff>
--- a/documentation/Flawless_QA_Usecases.xlsx
+++ b/documentation/Flawless_QA_Usecases.xlsx
@@ -5,15 +5,16 @@
   <workbookPr defaultThemeVersion="153222"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Teejay Hidalgo\Desktop\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\xampp\htdocs\flawless\documentation\"/>
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="20460" windowHeight="7170"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="20460" windowHeight="7170" activeTab="1"/>
   </bookViews>
   <sheets>
-    <sheet name="Testimonial_Manager" sheetId="1" r:id="rId1"/>
-    <sheet name="Status" sheetId="2" r:id="rId2"/>
+    <sheet name="Branch_Manager" sheetId="4" r:id="rId1"/>
+    <sheet name="Testimonial_Manager" sheetId="1" r:id="rId2"/>
+    <sheet name="Status" sheetId="2" r:id="rId3"/>
   </sheets>
   <calcPr calcId="152511"/>
   <extLst>
@@ -25,7 +26,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="32" uniqueCount="25">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="67" uniqueCount="27">
   <si>
     <t>User Cases</t>
   </si>
@@ -90,9 +91,6 @@
     <t>Click checkbox of random 2-3 items then on actions dropdown on top left select Delete and submit, un success refresh, items deleted should not show anymore</t>
   </si>
   <si>
-    <t>General notes, please make sure to refresh page after updates to make sure that changes are applied on database and not just a javascript effect. Make sure labels, breadcrumbs, notification messages are correct per module.</t>
-  </si>
-  <si>
     <t>Last Date Checked</t>
   </si>
   <si>
@@ -100,6 +98,15 @@
   </si>
   <si>
     <t>Teejay Hidalgo</t>
+  </si>
+  <si>
+    <t>General notes, please make sure to refresh page after updates to make sure that changes are applied on database and not just a javascript effect.</t>
+  </si>
+  <si>
+    <t>Make sure labels, breadcrumbs, notification messages are correct per module.</t>
+  </si>
+  <si>
+    <t>Especially for duplicated modules,  labels, error or success message may still carry out the original modules</t>
   </si>
 </sst>
 </file>
@@ -155,7 +162,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="6">
+  <cellXfs count="7">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment wrapText="1"/>
@@ -170,6 +177,9 @@
       <alignment wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="1" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="14" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyAlignment="1">
       <alignment wrapText="1"/>
     </xf>
   </cellXfs>
@@ -452,10 +462,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:E19"/>
+  <dimension ref="A1:E21"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="C4" sqref="C4"/>
+    <sheetView topLeftCell="B16" workbookViewId="0">
+      <selection activeCell="B30" sqref="B30"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="38.28515625" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -465,10 +475,10 @@
   <sheetData>
     <row r="1" spans="1:5" s="3" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A1" s="4" t="s">
+        <v>22</v>
+      </c>
+      <c r="B1" s="3" t="s">
         <v>23</v>
-      </c>
-      <c r="B1" s="3" t="s">
-        <v>24</v>
       </c>
     </row>
     <row r="3" spans="1:5" s="2" customFormat="1" x14ac:dyDescent="0.25">
@@ -485,12 +495,12 @@
         <v>1</v>
       </c>
       <c r="E3" s="5" t="s">
-        <v>22</v>
-      </c>
-    </row>
-    <row r="5" spans="1:5" ht="90" x14ac:dyDescent="0.25">
+        <v>21</v>
+      </c>
+    </row>
+    <row r="5" spans="1:5" ht="60" x14ac:dyDescent="0.25">
       <c r="B5" s="1" t="s">
-        <v>21</v>
+        <v>24</v>
       </c>
     </row>
     <row r="7" spans="1:5" x14ac:dyDescent="0.25">
@@ -503,6 +513,9 @@
       <c r="D7" s="1" t="s">
         <v>8</v>
       </c>
+      <c r="E7" s="6">
+        <v>42462</v>
+      </c>
     </row>
     <row r="9" spans="1:5" ht="30" x14ac:dyDescent="0.25">
       <c r="A9" s="1" t="s">
@@ -514,6 +527,9 @@
       <c r="D9" s="1" t="s">
         <v>8</v>
       </c>
+      <c r="E9" s="6">
+        <v>42462</v>
+      </c>
     </row>
     <row r="11" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A11" s="1" t="s">
@@ -525,6 +541,9 @@
       <c r="D11" s="1" t="s">
         <v>8</v>
       </c>
+      <c r="E11" s="6">
+        <v>42462</v>
+      </c>
     </row>
     <row r="13" spans="1:5" ht="60" x14ac:dyDescent="0.25">
       <c r="A13" s="1" t="s">
@@ -536,6 +555,9 @@
       <c r="D13" s="1" t="s">
         <v>8</v>
       </c>
+      <c r="E13" s="6">
+        <v>42462</v>
+      </c>
     </row>
     <row r="15" spans="1:5" ht="60" x14ac:dyDescent="0.25">
       <c r="A15" s="1" t="s">
@@ -547,8 +569,11 @@
       <c r="D15" s="1" t="s">
         <v>8</v>
       </c>
-    </row>
-    <row r="17" spans="1:4" ht="45" x14ac:dyDescent="0.25">
+      <c r="E15" s="6">
+        <v>42462</v>
+      </c>
+    </row>
+    <row r="17" spans="1:5" ht="45" x14ac:dyDescent="0.25">
       <c r="A17" s="1" t="s">
         <v>17</v>
       </c>
@@ -558,8 +583,11 @@
       <c r="D17" s="1" t="s">
         <v>8</v>
       </c>
-    </row>
-    <row r="19" spans="1:4" ht="60" x14ac:dyDescent="0.25">
+      <c r="E17" s="6">
+        <v>42462</v>
+      </c>
+    </row>
+    <row r="19" spans="1:5" ht="60" x14ac:dyDescent="0.25">
       <c r="A19" s="1" t="s">
         <v>18</v>
       </c>
@@ -568,6 +596,23 @@
       </c>
       <c r="D19" s="1" t="s">
         <v>8</v>
+      </c>
+      <c r="E19" s="6">
+        <v>42462</v>
+      </c>
+    </row>
+    <row r="21" spans="1:5" ht="45" x14ac:dyDescent="0.25">
+      <c r="A21" s="1" t="s">
+        <v>25</v>
+      </c>
+      <c r="B21" s="1" t="s">
+        <v>26</v>
+      </c>
+      <c r="D21" s="1" t="s">
+        <v>8</v>
+      </c>
+      <c r="E21" s="6">
+        <v>42462</v>
       </c>
     </row>
   </sheetData>
@@ -590,6 +635,179 @@
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+  <dimension ref="A1:E21"/>
+  <sheetViews>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="E24" sqref="E24"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultColWidth="38.28515625" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <cols>
+    <col min="1" max="16384" width="38.28515625" style="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:5" s="3" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A1" s="4" t="s">
+        <v>22</v>
+      </c>
+      <c r="B1" s="3" t="s">
+        <v>23</v>
+      </c>
+    </row>
+    <row r="3" spans="1:5" s="2" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A3" s="5" t="s">
+        <v>0</v>
+      </c>
+      <c r="B3" s="5" t="s">
+        <v>4</v>
+      </c>
+      <c r="C3" s="5" t="s">
+        <v>2</v>
+      </c>
+      <c r="D3" s="5" t="s">
+        <v>1</v>
+      </c>
+      <c r="E3" s="5" t="s">
+        <v>21</v>
+      </c>
+    </row>
+    <row r="5" spans="1:5" ht="60" x14ac:dyDescent="0.25">
+      <c r="B5" s="1" t="s">
+        <v>24</v>
+      </c>
+    </row>
+    <row r="7" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A7" s="1" t="s">
+        <v>3</v>
+      </c>
+      <c r="B7" s="1" t="s">
+        <v>5</v>
+      </c>
+      <c r="D7" s="1" t="s">
+        <v>8</v>
+      </c>
+      <c r="E7" s="6">
+        <v>42462</v>
+      </c>
+    </row>
+    <row r="9" spans="1:5" ht="30" x14ac:dyDescent="0.25">
+      <c r="A9" s="1" t="s">
+        <v>9</v>
+      </c>
+      <c r="B9" s="1" t="s">
+        <v>10</v>
+      </c>
+      <c r="D9" s="1" t="s">
+        <v>8</v>
+      </c>
+      <c r="E9" s="6">
+        <v>42462</v>
+      </c>
+    </row>
+    <row r="11" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A11" s="1" t="s">
+        <v>11</v>
+      </c>
+      <c r="B11" s="1" t="s">
+        <v>12</v>
+      </c>
+      <c r="D11" s="1" t="s">
+        <v>8</v>
+      </c>
+      <c r="E11" s="6">
+        <v>42462</v>
+      </c>
+    </row>
+    <row r="13" spans="1:5" ht="60" x14ac:dyDescent="0.25">
+      <c r="A13" s="1" t="s">
+        <v>13</v>
+      </c>
+      <c r="B13" s="1" t="s">
+        <v>15</v>
+      </c>
+      <c r="D13" s="1" t="s">
+        <v>8</v>
+      </c>
+      <c r="E13" s="6">
+        <v>42462</v>
+      </c>
+    </row>
+    <row r="15" spans="1:5" ht="60" x14ac:dyDescent="0.25">
+      <c r="A15" s="1" t="s">
+        <v>14</v>
+      </c>
+      <c r="B15" s="1" t="s">
+        <v>16</v>
+      </c>
+      <c r="D15" s="1" t="s">
+        <v>8</v>
+      </c>
+      <c r="E15" s="6">
+        <v>42462</v>
+      </c>
+    </row>
+    <row r="17" spans="1:5" ht="45" x14ac:dyDescent="0.25">
+      <c r="A17" s="1" t="s">
+        <v>17</v>
+      </c>
+      <c r="B17" s="1" t="s">
+        <v>19</v>
+      </c>
+      <c r="D17" s="1" t="s">
+        <v>8</v>
+      </c>
+      <c r="E17" s="6">
+        <v>42462</v>
+      </c>
+    </row>
+    <row r="19" spans="1:5" ht="60" x14ac:dyDescent="0.25">
+      <c r="A19" s="1" t="s">
+        <v>18</v>
+      </c>
+      <c r="B19" s="1" t="s">
+        <v>20</v>
+      </c>
+      <c r="D19" s="1" t="s">
+        <v>8</v>
+      </c>
+      <c r="E19" s="6">
+        <v>42462</v>
+      </c>
+    </row>
+    <row r="21" spans="1:5" ht="45" x14ac:dyDescent="0.25">
+      <c r="A21" s="1" t="s">
+        <v>25</v>
+      </c>
+      <c r="B21" s="1" t="s">
+        <v>26</v>
+      </c>
+      <c r="D21" s="1" t="s">
+        <v>8</v>
+      </c>
+      <c r="E21" s="6">
+        <v>42462</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageSetup orientation="portrait" horizontalDpi="4294967294" verticalDpi="0" r:id="rId1"/>
+  <extLst>
+    <ext xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" uri="{CCE6A557-97BC-4b89-ADB6-D9C93CAAB3DF}">
+      <x14:dataValidations xmlns:xm="http://schemas.microsoft.com/office/excel/2006/main" count="1">
+        <x14:dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1">
+          <x14:formula1>
+            <xm:f>Status!$A$1:$A$3</xm:f>
+          </x14:formula1>
+          <xm:sqref>D5:D108</xm:sqref>
+        </x14:dataValidation>
+      </x14:dataValidations>
+    </ext>
+  </extLst>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:A3"/>
   <sheetViews>
     <sheetView workbookViewId="0">

</xml_diff>